<commit_message>
update from home last commint
</commit_message>
<xml_diff>
--- a/SELBIETEST/MasterDataSheet.xlsx
+++ b/SELBIETEST/MasterDataSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>Serial</t>
   </si>
@@ -219,9 +219,6 @@
     <t>www.farmers.com</t>
   </si>
   <si>
-    <t>Training</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -229,6 +226,36 @@
   </si>
   <si>
     <t>exit</t>
+  </si>
+  <si>
+    <t>Describe Other</t>
+  </si>
+  <si>
+    <t>location address</t>
+  </si>
+  <si>
+    <t>additional address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>v@r.un</t>
+  </si>
+  <si>
+    <t>Training/Testing Quote</t>
+  </si>
+  <si>
+    <t>Maintained continous insurance coverage</t>
+  </si>
+  <si>
+    <t>543216545</t>
+  </si>
+  <si>
+    <t>15422541</t>
   </si>
 </sst>
 </file>
@@ -291,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -396,6 +423,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -404,7 +444,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -443,6 +483,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1211,8 +1261,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1418,42 +1468,45 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="29"/>
-    <col min="6" max="7" width="21.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="24" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="22" style="30" customWidth="1"/>
-    <col min="13" max="13" width="10" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="30" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" style="30" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="29" customWidth="1"/>
-    <col min="19" max="19" width="21.5703125" style="30" customWidth="1"/>
-    <col min="20" max="20" width="19" style="29" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="29"/>
-    <col min="22" max="22" width="17.42578125" style="29" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="29" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="29"/>
-    <col min="25" max="25" width="12.140625" style="29" customWidth="1"/>
-    <col min="26" max="26" width="12.28515625" style="29" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="28"/>
+    <col min="4" max="4" width="14.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="29"/>
+    <col min="7" max="8" width="21.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="24" style="29" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="29" customWidth="1"/>
+    <col min="17" max="18" width="22" style="30" customWidth="1"/>
+    <col min="19" max="19" width="16" style="29" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="30" customWidth="1"/>
+    <col min="23" max="24" width="22.42578125" style="30" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" style="29" customWidth="1"/>
+    <col min="26" max="26" width="21.5703125" style="30" customWidth="1"/>
+    <col min="27" max="27" width="19" style="29" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="29"/>
+    <col min="29" max="29" width="17.42578125" style="29" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" style="29" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="29"/>
+    <col min="32" max="32" width="12.140625" style="29" customWidth="1"/>
+    <col min="33" max="33" width="12.28515625" style="29" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" customFormat="1" ht="60.75" thickBot="1">
+    <row r="1" spans="1:35" customFormat="1" ht="60.75" thickBot="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1464,82 +1517,103 @@
         <v>30</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="P1" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="S1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="X1" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="AE1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AG1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AI1" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:28" customFormat="1">
+    <row r="2" spans="1:35" customFormat="1">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1549,81 +1623,90 @@
       <c r="C2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="P2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="19">
-        <v>15422541</v>
-      </c>
-      <c r="M2" s="19">
-        <v>543216545</v>
-      </c>
-      <c r="N2" s="31" t="s">
+      <c r="R2" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="19">
-        <v>2017</v>
-      </c>
-      <c r="R2" s="19">
-        <v>5</v>
-      </c>
-      <c r="S2" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="U2" s="19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="V2" s="19" t="s">
         <v>62</v>
       </c>
       <c r="W2" s="19">
-        <v>2</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>65</v>
-      </c>
+        <v>2017</v>
+      </c>
+      <c r="X2" s="19"/>
       <c r="Y2" s="19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z2" s="19" t="s">
         <v>62</v>
       </c>
       <c r="AA2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" s="19">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF2" s="19">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" customFormat="1">
+    </row>
+    <row r="3" spans="1:35" customFormat="1">
       <c r="A3" s="11"/>
       <c r="B3" s="24"/>
       <c r="C3" s="3"/>
@@ -1642,7 +1725,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="S3" s="34"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
@@ -1651,9 +1734,16 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="7"/>
-    </row>
-    <row r="4" spans="1:28" customFormat="1">
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="7"/>
+    </row>
+    <row r="4" spans="1:35" customFormat="1">
       <c r="A4" s="11"/>
       <c r="B4" s="24"/>
       <c r="C4" s="3"/>
@@ -1672,7 +1762,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="S4" s="34"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
@@ -1681,9 +1771,16 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="7"/>
-    </row>
-    <row r="5" spans="1:28" customFormat="1">
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="7"/>
+    </row>
+    <row r="5" spans="1:35" customFormat="1">
       <c r="A5" s="11"/>
       <c r="B5" s="24"/>
       <c r="C5" s="3"/>
@@ -1702,7 +1799,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="S5" s="34"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
@@ -1711,9 +1808,16 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="7"/>
-    </row>
-    <row r="6" spans="1:28" customFormat="1">
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="7"/>
+    </row>
+    <row r="6" spans="1:35" customFormat="1">
       <c r="A6" s="11"/>
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
@@ -1732,7 +1836,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="S6" s="34"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1741,9 +1845,16 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="7"/>
-    </row>
-    <row r="7" spans="1:28" customFormat="1">
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="7"/>
+    </row>
+    <row r="7" spans="1:35" customFormat="1">
       <c r="A7" s="11"/>
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
@@ -1762,7 +1873,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
+      <c r="S7" s="34"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1771,9 +1882,16 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="7"/>
-    </row>
-    <row r="8" spans="1:28" customFormat="1">
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="7"/>
+    </row>
+    <row r="8" spans="1:35" customFormat="1">
       <c r="A8" s="11"/>
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
@@ -1792,7 +1910,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="S8" s="34"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -1801,9 +1919,16 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="7"/>
-    </row>
-    <row r="9" spans="1:28" customFormat="1">
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="7"/>
+    </row>
+    <row r="9" spans="1:35" customFormat="1">
       <c r="A9" s="11"/>
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
@@ -1822,7 +1947,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="S9" s="34"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -1831,9 +1956,16 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="7"/>
-    </row>
-    <row r="10" spans="1:28" customFormat="1">
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="7"/>
+    </row>
+    <row r="10" spans="1:35" customFormat="1">
       <c r="A10" s="11"/>
       <c r="B10" s="24"/>
       <c r="C10" s="3"/>
@@ -1852,7 +1984,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="S10" s="34"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -1861,9 +1993,16 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="7"/>
-    </row>
-    <row r="11" spans="1:28" customFormat="1">
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="7"/>
+    </row>
+    <row r="11" spans="1:35" customFormat="1">
       <c r="A11" s="11"/>
       <c r="B11" s="24"/>
       <c r="C11" s="3"/>
@@ -1882,7 +2021,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="S11" s="34"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -1891,9 +2030,16 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="7"/>
-    </row>
-    <row r="12" spans="1:28" customFormat="1">
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="7"/>
+    </row>
+    <row r="12" spans="1:35" customFormat="1">
       <c r="A12" s="11"/>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
@@ -1912,7 +2058,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="S12" s="34"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -1921,9 +2067,16 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" customFormat="1">
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="7"/>
+    </row>
+    <row r="13" spans="1:35" customFormat="1">
       <c r="A13" s="11"/>
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
@@ -1942,7 +2095,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="S13" s="34"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -1951,9 +2104,16 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="7"/>
-    </row>
-    <row r="14" spans="1:28" customFormat="1">
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="7"/>
+    </row>
+    <row r="14" spans="1:35" customFormat="1">
       <c r="A14" s="11"/>
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
@@ -1972,7 +2132,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="S14" s="34"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -1981,9 +2141,16 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="7"/>
-    </row>
-    <row r="15" spans="1:28" customFormat="1">
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="7"/>
+    </row>
+    <row r="15" spans="1:35" customFormat="1">
       <c r="A15" s="11"/>
       <c r="B15" s="24"/>
       <c r="C15" s="3"/>
@@ -2002,7 +2169,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
+      <c r="S15" s="34"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -2011,9 +2178,16 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="7"/>
-    </row>
-    <row r="16" spans="1:28" customFormat="1">
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="7"/>
+    </row>
+    <row r="16" spans="1:35" customFormat="1">
       <c r="A16" s="11"/>
       <c r="B16" s="24"/>
       <c r="C16" s="3"/>
@@ -2032,7 +2206,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="S16" s="34"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -2041,9 +2215,16 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="7"/>
-    </row>
-    <row r="17" spans="1:28" customFormat="1">
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="7"/>
+    </row>
+    <row r="17" spans="1:35" customFormat="1">
       <c r="A17" s="11"/>
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
@@ -2062,7 +2243,7 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="S17" s="34"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -2071,9 +2252,16 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="7"/>
-    </row>
-    <row r="18" spans="1:28" customFormat="1">
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="7"/>
+    </row>
+    <row r="18" spans="1:35" customFormat="1">
       <c r="A18" s="11"/>
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
@@ -2092,7 +2280,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="S18" s="34"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -2101,9 +2289,16 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="7"/>
-    </row>
-    <row r="19" spans="1:28" customFormat="1">
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="7"/>
+    </row>
+    <row r="19" spans="1:35" customFormat="1">
       <c r="A19" s="11"/>
       <c r="B19" s="24"/>
       <c r="C19" s="3"/>
@@ -2122,7 +2317,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="34"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -2131,9 +2326,16 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="7"/>
-    </row>
-    <row r="20" spans="1:28" customFormat="1">
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="7"/>
+    </row>
+    <row r="20" spans="1:35" customFormat="1">
       <c r="A20" s="11"/>
       <c r="B20" s="24"/>
       <c r="C20" s="3"/>
@@ -2152,7 +2354,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="S20" s="34"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -2161,9 +2363,16 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
-      <c r="AB20" s="7"/>
-    </row>
-    <row r="21" spans="1:28" customFormat="1">
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="7"/>
+    </row>
+    <row r="21" spans="1:35" customFormat="1">
       <c r="A21" s="11"/>
       <c r="B21" s="24"/>
       <c r="C21" s="3"/>
@@ -2182,7 +2391,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="S21" s="34"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -2191,9 +2400,16 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
-      <c r="AB21" s="7"/>
-    </row>
-    <row r="22" spans="1:28" customFormat="1">
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="7"/>
+    </row>
+    <row r="22" spans="1:35" customFormat="1">
       <c r="A22" s="11"/>
       <c r="B22" s="24"/>
       <c r="C22" s="3"/>
@@ -2212,7 +2428,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="S22" s="34"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -2221,9 +2437,16 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="7"/>
-    </row>
-    <row r="23" spans="1:28" customFormat="1">
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="7"/>
+    </row>
+    <row r="23" spans="1:35" customFormat="1">
       <c r="A23" s="11"/>
       <c r="B23" s="24"/>
       <c r="C23" s="3"/>
@@ -2242,7 +2465,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+      <c r="S23" s="34"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2251,9 +2474,16 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="7"/>
-    </row>
-    <row r="24" spans="1:28" customFormat="1">
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="7"/>
+    </row>
+    <row r="24" spans="1:35" customFormat="1">
       <c r="A24" s="11"/>
       <c r="B24" s="24"/>
       <c r="C24" s="3"/>
@@ -2272,7 +2502,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
+      <c r="S24" s="34"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2281,9 +2511,16 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="7"/>
-    </row>
-    <row r="25" spans="1:28" customFormat="1">
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="7"/>
+    </row>
+    <row r="25" spans="1:35" customFormat="1">
       <c r="A25" s="11"/>
       <c r="B25" s="24"/>
       <c r="C25" s="3"/>
@@ -2302,7 +2539,7 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
+      <c r="S25" s="34"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -2311,9 +2548,16 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
-      <c r="AB25" s="7"/>
-    </row>
-    <row r="26" spans="1:28" customFormat="1">
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="7"/>
+    </row>
+    <row r="26" spans="1:35" customFormat="1">
       <c r="A26" s="11"/>
       <c r="B26" s="24"/>
       <c r="C26" s="3"/>
@@ -2332,7 +2576,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="S26" s="34"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2341,9 +2585,16 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
-      <c r="AB26" s="7"/>
-    </row>
-    <row r="27" spans="1:28" customFormat="1">
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="7"/>
+    </row>
+    <row r="27" spans="1:35" customFormat="1">
       <c r="A27" s="11"/>
       <c r="B27" s="24"/>
       <c r="C27" s="3"/>
@@ -2362,7 +2613,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="S27" s="34"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -2371,9 +2622,16 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
-      <c r="AB27" s="7"/>
-    </row>
-    <row r="28" spans="1:28" customFormat="1">
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="7"/>
+    </row>
+    <row r="28" spans="1:35" customFormat="1">
       <c r="A28" s="11"/>
       <c r="B28" s="24"/>
       <c r="C28" s="3"/>
@@ -2392,7 +2650,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
+      <c r="S28" s="34"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -2401,9 +2659,16 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="7"/>
-    </row>
-    <row r="29" spans="1:28" customFormat="1">
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="7"/>
+    </row>
+    <row r="29" spans="1:35" customFormat="1">
       <c r="A29" s="11"/>
       <c r="B29" s="24"/>
       <c r="C29" s="3"/>
@@ -2422,7 +2687,7 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
+      <c r="S29" s="34"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
@@ -2431,9 +2696,16 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="7"/>
-    </row>
-    <row r="30" spans="1:28" customFormat="1">
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="7"/>
+    </row>
+    <row r="30" spans="1:35" customFormat="1">
       <c r="A30" s="11"/>
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
@@ -2452,7 +2724,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
+      <c r="S30" s="34"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
@@ -2461,9 +2733,16 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
-      <c r="AB30" s="7"/>
-    </row>
-    <row r="31" spans="1:28" customFormat="1">
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="7"/>
+    </row>
+    <row r="31" spans="1:35" customFormat="1">
       <c r="A31" s="11"/>
       <c r="B31" s="24"/>
       <c r="C31" s="3"/>
@@ -2482,7 +2761,7 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
+      <c r="S31" s="34"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
@@ -2491,9 +2770,16 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
-      <c r="AB31" s="7"/>
-    </row>
-    <row r="32" spans="1:28" customFormat="1">
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="7"/>
+    </row>
+    <row r="32" spans="1:35" customFormat="1">
       <c r="A32" s="11"/>
       <c r="B32" s="24"/>
       <c r="C32" s="3"/>
@@ -2512,7 +2798,7 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
+      <c r="S32" s="34"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
@@ -2521,9 +2807,16 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
-      <c r="AB32" s="7"/>
-    </row>
-    <row r="33" spans="1:28" customFormat="1">
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="7"/>
+    </row>
+    <row r="33" spans="1:35" customFormat="1">
       <c r="A33" s="11"/>
       <c r="B33" s="24"/>
       <c r="C33" s="3"/>
@@ -2542,7 +2835,7 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
+      <c r="S33" s="34"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
@@ -2551,9 +2844,16 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
-      <c r="AB33" s="7"/>
-    </row>
-    <row r="34" spans="1:28" customFormat="1">
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="7"/>
+    </row>
+    <row r="34" spans="1:35" customFormat="1">
       <c r="A34" s="11"/>
       <c r="B34" s="24"/>
       <c r="C34" s="3"/>
@@ -2572,7 +2872,7 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
+      <c r="S34" s="34"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
@@ -2581,9 +2881,16 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
-      <c r="AB34" s="7"/>
-    </row>
-    <row r="35" spans="1:28" customFormat="1">
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="7"/>
+    </row>
+    <row r="35" spans="1:35" customFormat="1">
       <c r="A35" s="11"/>
       <c r="B35" s="24"/>
       <c r="C35" s="3"/>
@@ -2602,7 +2909,7 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
+      <c r="S35" s="34"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
@@ -2611,9 +2918,16 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
-      <c r="AB35" s="7"/>
-    </row>
-    <row r="36" spans="1:28" customFormat="1">
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
+      <c r="AG35" s="3"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="7"/>
+    </row>
+    <row r="36" spans="1:35" customFormat="1">
       <c r="A36" s="11"/>
       <c r="B36" s="24"/>
       <c r="C36" s="3"/>
@@ -2632,7 +2946,7 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
+      <c r="S36" s="34"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -2641,12 +2955,48 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
-      <c r="AB36" s="7"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="7"/>
+    </row>
+    <row r="37" spans="1:35">
+      <c r="S37" s="35"/>
+    </row>
+    <row r="38" spans="1:35">
+      <c r="S38" s="35"/>
+    </row>
+    <row r="39" spans="1:35">
+      <c r="S39" s="35"/>
+    </row>
+    <row r="40" spans="1:35">
+      <c r="S40" s="35"/>
+    </row>
+    <row r="41" spans="1:35">
+      <c r="S41" s="35"/>
+    </row>
+    <row r="42" spans="1:35">
+      <c r="S42" s="35"/>
+    </row>
+    <row r="43" spans="1:35">
+      <c r="S43" s="35"/>
+    </row>
+    <row r="44" spans="1:35">
+      <c r="S44" s="35"/>
+    </row>
+    <row r="45" spans="1:35">
+      <c r="S45" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId1"/>
+    <hyperlink ref="P2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>